<commit_message>
fixed mistake in layout
</commit_message>
<xml_diff>
--- a/simulation_model/stations.xlsx
+++ b/simulation_model/stations.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dav\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Farshid\Desktop\thesis\early-fault-detection\simulation_model\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22155" windowHeight="8580"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22160" windowHeight="8580"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -143,7 +143,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -304,14 +304,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -322,19 +316,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hivatkozás" xfId="1" builtinId="8"/>
-    <cellStyle name="Normál" xfId="0" builtinId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -677,17 +677,17 @@
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="137.5703125" customWidth="1"/>
-    <col min="9" max="9" width="47.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="103.453125" customWidth="1"/>
+    <col min="9" max="9" width="47.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>15</v>
@@ -714,7 +714,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -743,7 +743,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -769,7 +769,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -798,7 +798,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -824,7 +824,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
@@ -846,14 +846,14 @@
       <c r="G6" s="1">
         <v>1</v>
       </c>
-      <c r="H6" s="19" t="s">
+      <c r="H6" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="I6" s="23" t="s">
+      <c r="I6" s="20" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
@@ -869,10 +869,10 @@
         <v>1</v>
       </c>
       <c r="G7" s="1"/>
-      <c r="H7" s="20"/>
-      <c r="I7" s="22"/>
-    </row>
-    <row r="8" spans="1:9" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H7" s="18"/>
+      <c r="I7" s="21"/>
+    </row>
+    <row r="8" spans="1:9" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
@@ -888,10 +888,10 @@
       <c r="G8" s="1">
         <v>1</v>
       </c>
-      <c r="H8" s="21"/>
-      <c r="I8" s="22"/>
-    </row>
-    <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H8" s="19"/>
+      <c r="I8" s="21"/>
+    </row>
+    <row r="9" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="7" t="s">
         <v>7</v>
       </c>
@@ -917,7 +917,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A10" s="9" t="s">
         <v>8</v>
       </c>
@@ -943,7 +943,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="6" t="s">
         <v>9</v>
       </c>
@@ -954,14 +954,16 @@
         <v>0.5</v>
       </c>
       <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
+      <c r="E11" s="3">
+        <v>0.5</v>
+      </c>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
-      <c r="H11" s="16" t="s">
+      <c r="H11" s="22" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="6" t="s">
         <v>10</v>
       </c>
@@ -973,13 +975,13 @@
       </c>
       <c r="D12" s="3"/>
       <c r="E12" s="3">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
-      <c r="H12" s="18"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H12" s="23"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
@@ -1001,11 +1003,11 @@
       <c r="G13" s="1">
         <v>2</v>
       </c>
-      <c r="H13" s="16" t="s">
+      <c r="H13" s="22" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="6" t="s">
         <v>12</v>
       </c>
@@ -1027,9 +1029,9 @@
       <c r="G14" s="3">
         <v>0.5</v>
       </c>
-      <c r="H14" s="17"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H14" s="24"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="6" t="s">
         <v>13</v>
       </c>
@@ -1051,9 +1053,9 @@
       <c r="G15" s="3">
         <v>0.5</v>
       </c>
-      <c r="H15" s="18"/>
-    </row>
-    <row r="16" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="H15" s="23"/>
+    </row>
+    <row r="16" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
@@ -1075,11 +1077,11 @@
       <c r="G16" s="1">
         <v>1</v>
       </c>
-      <c r="H16" s="24" t="s">
+      <c r="H16" s="16" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
         <v>22</v>
       </c>
@@ -1108,7 +1110,7 @@
       </c>
       <c r="H17" s="13"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
         <v>21</v>
       </c>

</xml_diff>